<commit_message>
Update tekstdoc, update extraregels
</commit_message>
<xml_diff>
--- a/2. objectcatalogus/IMKL2015 v 1.0RC1plus-object-attributen-ExtraRegels.xlsx
+++ b/2. objectcatalogus/IMKL2015 v 1.0RC1plus-object-attributen-ExtraRegels.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="17175" windowHeight="7125" tabRatio="875" firstSheet="21" activeTab="29"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="17175" windowHeight="7125" tabRatio="875" firstSheet="11" activeTab="11"/>
   </bookViews>
   <sheets>
     <sheet name="IMKL2.2ExtraRegels" sheetId="23" state="hidden" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="336">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3542" uniqueCount="337">
   <si>
     <t>IMKL2.2 Extra regels</t>
   </si>
@@ -2242,6 +2242,9 @@
 • urn:ogc:def:uom:OGC::cm
 • urn:ogc:def:uom:OGC::mm</t>
   </si>
+  <si>
+    <t>Deze info zit al in de UtilityLinkSet. Op niveau van de individuele link is dit niet meer nodig. Wordt bijgevolg genegeerd als toch meegegeven wordt.</t>
+  </si>
 </sst>
 </file>
 
@@ -2367,7 +2370,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2404,6 +2407,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2863,7 +2872,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3050,6 +3059,12 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5349,8 +5364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -11659,8 +11674,8 @@
   </sheetPr>
   <dimension ref="A1:F30"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="110" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -11779,7 +11794,7 @@
       <c r="E6" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="78" t="s">
         <v>225</v>
       </c>
     </row>
@@ -11799,7 +11814,7 @@
       <c r="E7" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="F7" s="26" t="s">
+      <c r="F7" s="79" t="s">
         <v>226</v>
       </c>
     </row>
@@ -13866,8 +13881,8 @@
   </sheetPr>
   <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A3" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -14083,7 +14098,7 @@
         <v>131</v>
       </c>
       <c r="F11" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="36" customFormat="1">
@@ -14103,7 +14118,7 @@
         <v>131</v>
       </c>
       <c r="F12" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="36" customFormat="1">
@@ -14123,7 +14138,7 @@
         <v>131</v>
       </c>
       <c r="F13" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="36" customFormat="1">
@@ -14143,7 +14158,7 @@
         <v>131</v>
       </c>
       <c r="F14" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="36" customFormat="1">
@@ -14163,7 +14178,7 @@
         <v>137</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="36" customFormat="1">
@@ -14183,7 +14198,7 @@
         <v>137</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -14211,8 +14226,8 @@
   </sheetPr>
   <dimension ref="A1:F13"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -14374,7 +14389,7 @@
         <v>131</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="1" customFormat="1">
@@ -14394,7 +14409,7 @@
         <v>131</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -14414,7 +14429,7 @@
         <v>131</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="1" customFormat="1">
@@ -14434,7 +14449,7 @@
         <v>131</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -14454,7 +14469,7 @@
         <v>137</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1">
@@ -14474,7 +14489,7 @@
         <v>137</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>285</v>
+        <v>336</v>
       </c>
     </row>
   </sheetData>
@@ -14514,7 +14529,7 @@
   </sheetPr>
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScaleNormal="100" zoomScaleSheetLayoutView="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>

</xml_diff>